<commit_message>
Tests for 1904 Excel Dates
</commit_message>
<xml_diff>
--- a/test/Table_Tests/data/OlderDates1904.xlsx
+++ b/test/Table_Tests/data/OlderDates1904.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Repos\Enso\ide\test\Table_Tests\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{34FAE4A9-ECCA-48D0-AB68-36662EFAF76F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A1A84D3A-BAA0-42B0-B6C0-4F4E3869966B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="1140" yWindow="-15060" windowWidth="21600" windowHeight="11175" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -332,7 +332,7 @@
   <dimension ref="A1:E16"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A11" sqref="A11"/>
+      <selection activeCell="E2" sqref="E2:E16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="12.6328125" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
@@ -375,8 +375,7 @@
         <v>-3.4583333333333335</v>
       </c>
       <c r="E2" s="7">
-        <f ca="1">TIME(RANDBETWEEN(0,23),RANDBETWEEN(0,59),RANDBETWEEN(0,59))</f>
-        <v>0.2268287037037037</v>
+        <v>0.62212962962962959</v>
       </c>
     </row>
     <row r="3" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
@@ -397,8 +396,7 @@
         <v>-2.4583333333333335</v>
       </c>
       <c r="E3" s="7">
-        <f t="shared" ref="E3:E16" ca="1" si="4">TIME(RANDBETWEEN(0,23),RANDBETWEEN(0,59),RANDBETWEEN(0,59))</f>
-        <v>0.85173611111111114</v>
+        <v>0.43752314814814813</v>
       </c>
     </row>
     <row r="4" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
@@ -419,8 +417,7 @@
         <v>-1.4583333333333335</v>
       </c>
       <c r="E4" s="7">
-        <f t="shared" ca="1" si="4"/>
-        <v>6.9907407407407404E-2</v>
+        <v>0.96317129629629628</v>
       </c>
     </row>
     <row r="5" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
@@ -441,8 +438,7 @@
         <v>-0.45833333333333337</v>
       </c>
       <c r="E5" s="7">
-        <f t="shared" ca="1" si="4"/>
-        <v>0.70121527777777781</v>
+        <v>0.65208333333333335</v>
       </c>
     </row>
     <row r="6" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
@@ -462,8 +458,7 @@
         <v>0.54166666666666663</v>
       </c>
       <c r="E6" s="7">
-        <f t="shared" ca="1" si="4"/>
-        <v>0.75429398148148152</v>
+        <v>6.7604166666666674E-2</v>
       </c>
     </row>
     <row r="7" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
@@ -484,8 +479,7 @@
         <v>1.5416666666666665</v>
       </c>
       <c r="E7" s="7">
-        <f t="shared" ca="1" si="4"/>
-        <v>0.6125694444444445</v>
+        <v>0.71983796296296299</v>
       </c>
     </row>
     <row r="8" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
@@ -506,8 +500,7 @@
         <v>2.5416666666666665</v>
       </c>
       <c r="E8" s="7">
-        <f t="shared" ca="1" si="4"/>
-        <v>0.70571759259259259</v>
+        <v>0.43186342592592591</v>
       </c>
     </row>
     <row r="9" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
@@ -528,8 +521,7 @@
         <v>3.5416666666666665</v>
       </c>
       <c r="E9" s="7">
-        <f t="shared" ca="1" si="4"/>
-        <v>0.88782407407407404</v>
+        <v>0.10357638888888888</v>
       </c>
     </row>
     <row r="10" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
@@ -550,8 +542,7 @@
         <v>4.541666666666667</v>
       </c>
       <c r="E10" s="7">
-        <f t="shared" ca="1" si="4"/>
-        <v>0.24048611111111112</v>
+        <v>0.43119212962962961</v>
       </c>
     </row>
     <row r="11" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
@@ -571,13 +562,12 @@
         <v>59.541666666666664</v>
       </c>
       <c r="E11" s="7">
-        <f t="shared" ca="1" si="4"/>
-        <v>0.9816435185185185</v>
+        <v>9.087962962962963E-2</v>
       </c>
     </row>
     <row r="12" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A12" s="3">
-        <f t="shared" ref="A12:A16" si="5">A11+1</f>
+        <f t="shared" ref="A12:A16" si="4">A11+1</f>
         <v>60</v>
       </c>
       <c r="B12" s="4">
@@ -593,13 +583,12 @@
         <v>60.541666666666664</v>
       </c>
       <c r="E12" s="7">
-        <f t="shared" ca="1" si="4"/>
-        <v>0.74750000000000005</v>
+        <v>0.32666666666666666</v>
       </c>
     </row>
     <row r="13" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A13" s="3">
-        <f t="shared" si="5"/>
+        <f t="shared" si="4"/>
         <v>61</v>
       </c>
       <c r="B13" s="4">
@@ -615,13 +604,12 @@
         <v>61.541666666666664</v>
       </c>
       <c r="E13" s="7">
-        <f t="shared" ca="1" si="4"/>
-        <v>0.58733796296296292</v>
+        <v>0.24042824074074073</v>
       </c>
     </row>
     <row r="14" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A14" s="3">
-        <f t="shared" si="5"/>
+        <f t="shared" si="4"/>
         <v>62</v>
       </c>
       <c r="B14" s="4">
@@ -637,13 +625,12 @@
         <v>62.541666666666664</v>
       </c>
       <c r="E14" s="7">
-        <f t="shared" ca="1" si="4"/>
-        <v>0.83638888888888885</v>
+        <v>0.77543981481481483</v>
       </c>
     </row>
     <row r="15" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A15" s="3">
-        <f t="shared" si="5"/>
+        <f t="shared" si="4"/>
         <v>63</v>
       </c>
       <c r="B15" s="4">
@@ -659,13 +646,12 @@
         <v>63.541666666666664</v>
       </c>
       <c r="E15" s="7">
-        <f t="shared" ca="1" si="4"/>
-        <v>0.7855092592592593</v>
+        <v>0.64909722222222221</v>
       </c>
     </row>
     <row r="16" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A16" s="3">
-        <f t="shared" si="5"/>
+        <f t="shared" si="4"/>
         <v>64</v>
       </c>
       <c r="B16" s="4">
@@ -681,8 +667,7 @@
         <v>64.541666666666671</v>
       </c>
       <c r="E16" s="7">
-        <f t="shared" ca="1" si="4"/>
-        <v>0.85263888888888884</v>
+        <v>0.35109953703703706</v>
       </c>
     </row>
   </sheetData>

</xml_diff>